<commit_message>
AutoDS Validation / non-régression (suite Pandas 1.1.2 : variations bizarres résultats analyses de réf. 9 et 30 déjà problématiques sensibilité ordre)
</commit_message>
<xml_diff>
--- a/autods/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
+++ b/autods/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-sandbox\perso\AutoDS\refout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A4CAF4-FE04-412B-A5BA-52EB3385AE11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F040D75-2368-4618-AC9F-4E1A64CECB71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="9564" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="25848" windowHeight="15864" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats" sheetId="7" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -662,7 +665,7 @@
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,8 +1193,8 @@
         <v>423</v>
       </c>
       <c r="N7" s="10">
-        <f>O7-O10</f>
-        <v>178.79500000000007</v>
+        <f>O7-O9</f>
+        <v>10.139999999999418</v>
       </c>
       <c r="O7">
         <v>4658.1239999999998</v>
@@ -1277,8 +1280,8 @@
         <v>423</v>
       </c>
       <c r="N8" s="10">
-        <f>O8-O10</f>
-        <v>178.79500000000007</v>
+        <f>O8-O9</f>
+        <v>10.139999999999418</v>
       </c>
       <c r="O8">
         <v>4658.1239999999998</v>
@@ -1364,8 +1367,8 @@
         <v>423</v>
       </c>
       <c r="N9" s="10">
-        <f>O9-O10</f>
-        <v>168.65500000000065</v>
+        <f>O9-O9</f>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>4647.9840000000004</v>
@@ -1541,8 +1544,8 @@
         <v>423</v>
       </c>
       <c r="N11" s="10">
-        <f>O11-O10</f>
-        <v>235.15500000000065</v>
+        <f>O11-O9</f>
+        <v>66.5</v>
       </c>
       <c r="O11">
         <v>4714.4840000000004</v>
@@ -1651,8 +1654,8 @@
         <v>423</v>
       </c>
       <c r="N13">
-        <f>O13-O16</f>
-        <v>574.41599999999971</v>
+        <f>O13-O15</f>
+        <v>10.127999999999702</v>
       </c>
       <c r="O13">
         <v>4658.0529999999999</v>
@@ -1738,8 +1741,8 @@
         <v>423</v>
       </c>
       <c r="N14">
-        <f>O14-O16</f>
-        <v>574.41599999999971</v>
+        <f>O14-O15</f>
+        <v>10.127999999999702</v>
       </c>
       <c r="O14">
         <v>4658.0529999999999</v>
@@ -1825,8 +1828,8 @@
         <v>423</v>
       </c>
       <c r="N15">
-        <f>O15-O16</f>
-        <v>564.28800000000001</v>
+        <f>O15-O15</f>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>4647.9250000000002</v>
@@ -2007,8 +2010,8 @@
         <v>423</v>
       </c>
       <c r="N17">
-        <f>O17-O16</f>
-        <v>630.78400000000011</v>
+        <f>O17-O15</f>
+        <v>66.496000000000095</v>
       </c>
       <c r="O17">
         <v>4714.4210000000003</v>
@@ -2117,8 +2120,8 @@
         <v>217</v>
       </c>
       <c r="N19">
-        <f>O19-O22</f>
-        <v>1777.3537000000001</v>
+        <f>O19-O19</f>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>2318.1190000000001</v>
@@ -2204,8 +2207,8 @@
         <v>217</v>
       </c>
       <c r="N20">
-        <f>O20-O22</f>
-        <v>1777.3537000000001</v>
+        <f>O20-O19</f>
+        <v>0</v>
       </c>
       <c r="O20">
         <v>2318.1190000000001</v>
@@ -2296,8 +2299,8 @@
         <v>215</v>
       </c>
       <c r="N21">
-        <f>O21-O22</f>
-        <v>1729.3157000000001</v>
+        <f>O21-O21</f>
+        <v>0</v>
       </c>
       <c r="O21" s="10">
         <v>2270.0810000000001</v>
@@ -2474,8 +2477,8 @@
         <v>217</v>
       </c>
       <c r="N23">
-        <f>O23-O22</f>
-        <v>1786.8427000000001</v>
+        <f>O23-O19</f>
+        <v>9.4890000000000327</v>
       </c>
       <c r="O23">
         <v>2327.6080000000002</v>
@@ -2561,8 +2564,8 @@
         <v>217</v>
       </c>
       <c r="N24">
-        <f>O24-O22</f>
-        <v>1777.3737000000001</v>
+        <f>O24-O19</f>
+        <v>1.999999999998181E-2</v>
       </c>
       <c r="O24">
         <v>2318.1390000000001</v>
@@ -2648,8 +2651,8 @@
         <v>217</v>
       </c>
       <c r="N25">
-        <f>O25-O22</f>
-        <v>1777.9607000000001</v>
+        <f>O25-O19</f>
+        <v>0.6069999999999709</v>
       </c>
       <c r="O25">
         <v>2318.7260000000001</v>
@@ -2735,8 +2738,8 @@
         <v>217</v>
       </c>
       <c r="N26">
-        <f>O26-O30</f>
-        <v>1777.3522000000003</v>
+        <f>O26-O26</f>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>2318.1170000000002</v>
@@ -2919,8 +2922,8 @@
         <v>217</v>
       </c>
       <c r="N28">
-        <f>O28-O30</f>
-        <v>1777.3522000000003</v>
+        <f>O28-O26</f>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>2318.1170000000002</v>
@@ -3189,8 +3192,8 @@
         <v>217</v>
       </c>
       <c r="N31">
-        <f>O31-O30</f>
-        <v>1778.8812000000003</v>
+        <f>O31-O26</f>
+        <v>1.5289999999999964</v>
       </c>
       <c r="O31">
         <v>2319.6460000000002</v>
@@ -3276,8 +3279,8 @@
         <v>217</v>
       </c>
       <c r="N32">
-        <f>O32-O30</f>
-        <v>1777.3591999999999</v>
+        <f>O32-O26</f>
+        <v>6.9999999996070983E-3</v>
       </c>
       <c r="O32">
         <v>2318.1239999999998</v>
@@ -3363,8 +3366,8 @@
         <v>217</v>
       </c>
       <c r="N33">
-        <f>O33-O30</f>
-        <v>1777.9572000000003</v>
+        <f>O33-O26</f>
+        <v>0.60500000000001819</v>
       </c>
       <c r="O33">
         <v>2318.7220000000002</v>

</xml_diff>